<commit_message>
data label updated, added package
and z-score in univariate boxplots
</commit_message>
<xml_diff>
--- a/SystemSerology_MachineLearning/RSTR_data_NatureMedicine.xlsx
+++ b/SystemSerology_MachineLearning/RSTR_data_NatureMedicine.xlsx
@@ -1707,7 +1707,7 @@
         <v>61.92374587168514</v>
       </c>
       <c r="ED2">
-        <v>29.99550526665494</v>
+        <v>29.99550526665495</v>
       </c>
       <c r="EE2">
         <v>40.99196810693557</v>
@@ -2038,10 +2038,10 @@
         <v>0.5686619718309859</v>
       </c>
       <c r="BB3">
-        <v>1.285106382978723</v>
+        <v>1.285106382978724</v>
       </c>
       <c r="BC3">
-        <v>1.69047619047619</v>
+        <v>1.690476190476191</v>
       </c>
       <c r="BD3">
         <v>0.7755775577557755</v>
@@ -2272,7 +2272,7 @@
         <v>43.15494803299681</v>
       </c>
       <c r="EB3">
-        <v>45.07281336549629</v>
+        <v>45.0728133654963</v>
       </c>
       <c r="EC3">
         <v>65.36823609994342</v>
@@ -2600,7 +2600,7 @@
         <v>29.18828451882845</v>
       </c>
       <c r="AY4">
-        <v>88.86624203821655</v>
+        <v>88.86624203821656</v>
       </c>
       <c r="AZ4">
         <v>45.37235772357724</v>
@@ -2609,7 +2609,7 @@
         <v>0.2598784194528875</v>
       </c>
       <c r="BB4">
-        <v>0.6129707112970711</v>
+        <v>0.6129707112970712</v>
       </c>
       <c r="BC4">
         <v>4.191082802547771</v>
@@ -2918,7 +2918,7 @@
         <v>1.631756801178126</v>
       </c>
       <c r="FA4">
-        <v>0.4036658645944275</v>
+        <v>0.4036658645944276</v>
       </c>
       <c r="FB4">
         <v>0.7784045336804597</v>
@@ -3014,7 +3014,7 @@
         <v>18.78</v>
       </c>
       <c r="GG4">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="5">
@@ -3159,7 +3159,7 @@
         <v>150.5</v>
       </c>
       <c r="AU5">
-        <v>8.008746355685131</v>
+        <v>8.008746355685132</v>
       </c>
       <c r="AV5">
         <v>106.2254237288136</v>
@@ -3417,7 +3417,7 @@
         <v>43.47794649313088</v>
       </c>
       <c r="EC5">
-        <v>76.42805495300072</v>
+        <v>76.42805495300073</v>
       </c>
       <c r="ED5">
         <v>31.91612436731743</v>
@@ -3480,7 +3480,7 @@
         <v>0.6097854904796337</v>
       </c>
       <c r="EX5">
-        <v>3.832248734634851</v>
+        <v>3.832248734634852</v>
       </c>
       <c r="EY5">
         <v>4.784285369968668</v>
@@ -3489,10 +3489,10 @@
         <v>2.171607616293083</v>
       </c>
       <c r="FA5">
-        <v>0.5109664979513135</v>
+        <v>0.5109664979513136</v>
       </c>
       <c r="FB5">
-        <v>8.667148710532659</v>
+        <v>8.66714871053266</v>
       </c>
       <c r="FC5">
         <v>6.329235960472403</v>
@@ -3513,7 +3513,7 @@
         <v>31.54</v>
       </c>
       <c r="FI5">
-        <v>93.64000000000001</v>
+        <v>93.64000000000002</v>
       </c>
       <c r="FJ5">
         <v>8.59</v>
@@ -3745,7 +3745,7 @@
         <v>227.7559523809524</v>
       </c>
       <c r="AZ6">
-        <v>134.9664902998236</v>
+        <v>134.9664902998237</v>
       </c>
       <c r="BA6">
         <v>0.3100081366965012</v>
@@ -4036,7 +4036,7 @@
         <v>0.3560299953770136</v>
       </c>
       <c r="ES6">
-        <v>2.599679392887805</v>
+        <v>2.599679392887806</v>
       </c>
       <c r="ET6">
         <v>0.4863141589466795</v>
@@ -4244,7 +4244,7 @@
         <v>4.395061728395062</v>
       </c>
       <c r="BD7">
-        <v>3.048092868988391</v>
+        <v>3.048092868988392</v>
       </c>
       <c r="BE7">
         <v>73005140</v>
@@ -4968,7 +4968,7 @@
         <v>16.46474054858675</v>
       </c>
       <c r="EE8">
-        <v>24.7678821696249</v>
+        <v>24.76788216962491</v>
       </c>
       <c r="EF8">
         <v>23.8179966398844</v>
@@ -4992,7 +4992,7 @@
         <v>0.02419979630387284</v>
       </c>
       <c r="EM8">
-        <v>0.1960357599867684</v>
+        <v>0.1960357599867685</v>
       </c>
       <c r="EN8">
         <v>0.4559659461859206</v>
@@ -5052,7 +5052,7 @@
         <v>34.99</v>
       </c>
       <c r="FG8">
-        <v>36.37</v>
+        <v>36.37000000000001</v>
       </c>
       <c r="FH8">
         <v>28.66</v>
@@ -5106,7 +5106,7 @@
         <v>0.16</v>
       </c>
       <c r="FY8">
-        <v>3.79</v>
+        <v>3.790000000000001</v>
       </c>
       <c r="FZ8">
         <v>0.18</v>
@@ -5152,7 +5152,7 @@
         <v>0.92</v>
       </c>
       <c r="F9">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="G9">
         <v>14.7</v>
@@ -5557,7 +5557,7 @@
         <v>2.365448228514365</v>
       </c>
       <c r="EK9">
-        <v>2.945888031289658</v>
+        <v>2.945888031289659</v>
       </c>
       <c r="EL9">
         <v>2.208375808766929</v>
@@ -6095,7 +6095,7 @@
         <v>91633</v>
       </c>
       <c r="DZ10">
-        <v>15.62132298509323</v>
+        <v>15.62132298509324</v>
       </c>
       <c r="EA10">
         <v>34.58712236326375</v>
@@ -6116,7 +6116,7 @@
         <v>22.31573041587769</v>
       </c>
       <c r="EG10">
-        <v>48.61646835137262</v>
+        <v>48.61646835137263</v>
       </c>
       <c r="EH10">
         <v>3.991241399194271</v>
@@ -6155,7 +6155,7 @@
         <v>3.118498258409893</v>
       </c>
       <c r="ET10">
-        <v>1.344959518744496</v>
+        <v>1.344959518744497</v>
       </c>
       <c r="EU10">
         <v>2.981352907715205</v>
@@ -6200,7 +6200,7 @@
         <v>31.25</v>
       </c>
       <c r="FI10">
-        <v>93.98999999999999</v>
+        <v>93.99</v>
       </c>
       <c r="FJ10">
         <v>7.299999999999998</v>
@@ -6747,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="FA11">
-        <v>0.1136803471039931</v>
+        <v>0.1136803471039932</v>
       </c>
       <c r="FB11">
         <v>3.965820108970732</v>
@@ -6768,7 +6768,7 @@
         <v>37.15</v>
       </c>
       <c r="FH11">
-        <v>32.62</v>
+        <v>32.62000000000001</v>
       </c>
       <c r="FI11">
         <v>95.34999999999999</v>
@@ -6988,7 +6988,7 @@
         <v>146.5</v>
       </c>
       <c r="AU12">
-        <v>4.526627218934911</v>
+        <v>4.526627218934912</v>
       </c>
       <c r="AV12">
         <v>25.92765273311897</v>
@@ -6997,7 +6997,7 @@
         <v>2.936660268714011</v>
       </c>
       <c r="AX12">
-        <v>36.32207207207207</v>
+        <v>36.32207207207208</v>
       </c>
       <c r="AY12">
         <v>49.46932515337424</v>
@@ -7276,7 +7276,7 @@
         <v>1.444043321299639</v>
       </c>
       <c r="EM12">
-        <v>0.1122313462149978</v>
+        <v>0.1122313462149979</v>
       </c>
       <c r="EN12">
         <v>0.643459718299321</v>
@@ -7583,7 +7583,7 @@
         <v>1.151277013752456</v>
       </c>
       <c r="BC13">
-        <v>2.389438943894389</v>
+        <v>2.38943894389439</v>
       </c>
       <c r="BD13">
         <v>0.8399339933993399</v>
@@ -7880,7 +7880,7 @@
         <v>0.4291530346667537</v>
       </c>
       <c r="EX13">
-        <v>3.761208155539419</v>
+        <v>3.76120815553942</v>
       </c>
       <c r="EY13">
         <v>3.3157375149918</v>
@@ -7976,7 +7976,7 @@
         <v>8.970000000000001</v>
       </c>
       <c r="GD13">
-        <v>4.27</v>
+        <v>4.270000000000001</v>
       </c>
       <c r="GE13">
         <v>0.17</v>
@@ -8013,7 +8013,7 @@
         <v>9.970000000000001</v>
       </c>
       <c r="H14">
-        <v>76.53476999999999</v>
+        <v>76.53477</v>
       </c>
       <c r="I14">
         <v>53.654245</v>
@@ -8448,7 +8448,7 @@
         <v>1.730167921250724</v>
       </c>
       <c r="EW14">
-        <v>1.080486392588303</v>
+        <v>1.080486392588304</v>
       </c>
       <c r="EX14">
         <v>8.010422698320788</v>
@@ -8977,7 +8977,7 @@
         <v>2.401484937416911</v>
       </c>
       <c r="EI15">
-        <v>5.214839340808187</v>
+        <v>5.214839340808188</v>
       </c>
       <c r="EJ15">
         <v>0.1429753931823312</v>
@@ -9037,7 +9037,7 @@
         <v>2.823387764316352</v>
       </c>
       <c r="FC15">
-        <v>21.42774725963829</v>
+        <v>21.4277472596383</v>
       </c>
       <c r="FD15">
         <v>28.45511325156144</v>
@@ -9281,7 +9281,7 @@
         <v>2.708542713567839</v>
       </c>
       <c r="AX16">
-        <v>35.73998178506375</v>
+        <v>35.73998178506376</v>
       </c>
       <c r="AY16">
         <v>232.2041420118343</v>
@@ -9296,7 +9296,7 @@
         <v>0.2759562841530054</v>
       </c>
       <c r="BC16">
-        <v>1.766272189349112</v>
+        <v>1.766272189349113</v>
       </c>
       <c r="BD16">
         <v>2.299476439790576</v>
@@ -9521,7 +9521,7 @@
         <v>62063.25</v>
       </c>
       <c r="DZ16">
-        <v>14.58643001662693</v>
+        <v>14.58643001662694</v>
       </c>
       <c r="EA16">
         <v>21.6646968088303</v>
@@ -9542,7 +9542,7 @@
         <v>14.91856808029007</v>
       </c>
       <c r="EG16">
-        <v>61.53729041046495</v>
+        <v>61.53729041046496</v>
       </c>
       <c r="EH16">
         <v>5.730884032132054</v>
@@ -9572,7 +9572,7 @@
         <v>1.191530279052064</v>
       </c>
       <c r="EQ16">
-        <v>0.5577034796370119</v>
+        <v>0.557703479637012</v>
       </c>
       <c r="ER16">
         <v>2.130651655682205</v>
@@ -9602,19 +9602,19 @@
         <v>1.782888279012</v>
       </c>
       <c r="FA16">
-        <v>1.39906648771009</v>
+        <v>1.399066487710091</v>
       </c>
       <c r="FB16">
         <v>3.482441555319618</v>
       </c>
       <c r="FC16">
-        <v>8.152406899176666</v>
+        <v>8.152406899176667</v>
       </c>
       <c r="FD16">
         <v>19.64061780083736</v>
       </c>
       <c r="FE16">
-        <v>15.34325607484124</v>
+        <v>15.34325607484125</v>
       </c>
       <c r="FF16">
         <v>30.49</v>
@@ -9686,7 +9686,7 @@
         <v>26.79</v>
       </c>
       <c r="GC16">
-        <v>7.149999999999999</v>
+        <v>7.15</v>
       </c>
       <c r="GD16">
         <v>2.67</v>
@@ -9861,7 +9861,7 @@
         <v>37.45362563237774</v>
       </c>
       <c r="BA17">
-        <v>0.5858085808580858</v>
+        <v>0.5858085808580859</v>
       </c>
       <c r="BB17">
         <v>1.7</v>
@@ -10122,7 +10122,7 @@
         <v>6.385615838442598</v>
       </c>
       <c r="EJ17">
-        <v>0.6048487051940969</v>
+        <v>0.604848705194097</v>
       </c>
       <c r="EK17">
         <v>6.868172728925319</v>
@@ -10131,7 +10131,7 @@
         <v>1.804630563038125</v>
       </c>
       <c r="EM17">
-        <v>0.338781378592322</v>
+        <v>0.3387813785923221</v>
       </c>
       <c r="EN17">
         <v>0.3800961808596784</v>
@@ -10711,7 +10711,7 @@
         <v>13.31903641549897</v>
       </c>
       <c r="EP18">
-        <v>6.587686606008869</v>
+        <v>6.58768660600887</v>
       </c>
       <c r="EQ18">
         <v>5.584126257053031</v>
@@ -10768,7 +10768,7 @@
         <v>34.57999999999999</v>
       </c>
       <c r="FI18">
-        <v>85.48999999999999</v>
+        <v>85.49</v>
       </c>
       <c r="FJ18">
         <v>11.44</v>
@@ -10862,7 +10862,7 @@
         <v>0.51</v>
       </c>
       <c r="F19">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="G19">
         <v>14</v>
@@ -11258,7 +11258,7 @@
         <v>51.89062440906168</v>
       </c>
       <c r="EH19">
-        <v>4.266101887220604</v>
+        <v>4.266101887220605</v>
       </c>
       <c r="EI19">
         <v>11.23205123356404</v>
@@ -11306,7 +11306,7 @@
         <v>6.955863999092318</v>
       </c>
       <c r="EX19">
-        <v>4.076497358899688</v>
+        <v>4.076497358899689</v>
       </c>
       <c r="EY19">
         <v>6.919556748988313</v>
@@ -11490,7 +11490,7 @@
         <v>75.26344086021506</v>
       </c>
       <c r="BA20">
-        <v>0.5205254515599343</v>
+        <v>0.5205254515599344</v>
       </c>
       <c r="BB20">
         <v>1.029556650246305</v>
@@ -12334,7 +12334,7 @@
         <v>0.8756200239457523</v>
       </c>
       <c r="EN21">
-        <v>1.917867172801156</v>
+        <v>1.917867172801157</v>
       </c>
       <c r="EO21">
         <v>15.25024414736017</v>
@@ -12869,7 +12869,7 @@
         <v>38.86311637464113</v>
       </c>
       <c r="EB22">
-        <v>43.45796435458877</v>
+        <v>43.45796435458878</v>
       </c>
       <c r="EC22">
         <v>59.05003861829098</v>
@@ -14005,7 +14005,7 @@
         <v>58593.5</v>
       </c>
       <c r="DZ24">
-        <v>10.55646301355815</v>
+        <v>10.55646301355816</v>
       </c>
       <c r="EA24">
         <v>35.1523186569296</v>
@@ -14213,7 +14213,7 @@
         <v>83.86719000000001</v>
       </c>
       <c r="I25">
-        <v>67.00494</v>
+        <v>67.00494000000001</v>
       </c>
       <c r="J25">
         <v>6.82157</v>
@@ -14621,7 +14621,7 @@
         <v>0.7041223161051977</v>
       </c>
       <c r="EO25">
-        <v>16.26248216833095</v>
+        <v>16.26248216833096</v>
       </c>
       <c r="EP25">
         <v>9.237719009473645</v>
@@ -14636,7 +14636,7 @@
         <v>3.38344489557043</v>
       </c>
       <c r="ET25">
-        <v>4.956289549727495</v>
+        <v>4.956289549727496</v>
       </c>
       <c r="EU25">
         <v>8.743918943633638</v>
@@ -14711,7 +14711,7 @@
         <v>4.2</v>
       </c>
       <c r="FS25">
-        <v>7.399999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="FT25">
         <v>1.13</v>
@@ -15180,7 +15180,7 @@
         <v>4.727993274888916</v>
       </c>
       <c r="EK26">
-        <v>2.017533325327248</v>
+        <v>2.017533325327249</v>
       </c>
       <c r="EL26">
         <v>0</v>
@@ -15189,7 +15189,7 @@
         <v>1.246547376005764</v>
       </c>
       <c r="EN26">
-        <v>0.01561186501741323</v>
+        <v>0.01561186501741324</v>
       </c>
       <c r="EO26">
         <v>15.10748168608142</v>
@@ -15228,7 +15228,7 @@
         <v>1.066410471958689</v>
       </c>
       <c r="FA26">
-        <v>0.2341779752611985</v>
+        <v>0.2341779752611986</v>
       </c>
       <c r="FB26">
         <v>4.090308634562268</v>
@@ -15724,7 +15724,7 @@
         <v>30.66474912112496</v>
       </c>
       <c r="EB27">
-        <v>61.70574392050901</v>
+        <v>61.70574392050902</v>
       </c>
       <c r="EC27">
         <v>52.12092158400883</v>
@@ -15805,7 +15805,7 @@
         <v>3.412359452627909</v>
       </c>
       <c r="FC27">
-        <v>19.02437607135593</v>
+        <v>19.02437607135594</v>
       </c>
       <c r="FD27">
         <v>9.564484732269968</v>
@@ -15914,7 +15914,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="F28">
         <v>0.41</v>
@@ -16289,7 +16289,7 @@
         <v>62115</v>
       </c>
       <c r="DZ28">
-        <v>14.44041299917131</v>
+        <v>14.44041299917132</v>
       </c>
       <c r="EA28">
         <v>32.75325315236623</v>
@@ -16319,7 +16319,7 @@
         <v>6.828820354319245</v>
       </c>
       <c r="EJ28">
-        <v>0.8174875137181123</v>
+        <v>0.8174875137181124</v>
       </c>
       <c r="EK28">
         <v>3.886985150843244</v>
@@ -16328,7 +16328,7 @@
         <v>0.6271137091536204</v>
       </c>
       <c r="EM28">
-        <v>2.488297610248829</v>
+        <v>2.48829761024883</v>
       </c>
       <c r="EN28">
         <v>0.5285672691437658</v>
@@ -16397,7 +16397,7 @@
         <v>90.09000000000002</v>
       </c>
       <c r="FJ28">
-        <v>8.06</v>
+        <v>8.060000000000001</v>
       </c>
       <c r="FK28">
         <v>2.15</v>
@@ -16424,10 +16424,10 @@
         <v>4.34</v>
       </c>
       <c r="FS28">
-        <v>7.81</v>
+        <v>7.810000000000001</v>
       </c>
       <c r="FT28">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="FU28">
         <v>0.13</v>
@@ -16881,7 +16881,7 @@
         <v>21.54742399417441</v>
       </c>
       <c r="EG29">
-        <v>40.91753140360458</v>
+        <v>40.91753140360459</v>
       </c>
       <c r="EH29">
         <v>1.387220098306936</v>
@@ -16902,7 +16902,7 @@
         <v>1.867831785909339</v>
       </c>
       <c r="EN29">
-        <v>0.9393773894046969</v>
+        <v>0.939377389404697</v>
       </c>
       <c r="EO29">
         <v>21.6602949208083</v>
@@ -16923,7 +16923,7 @@
         <v>4.008738394320044</v>
       </c>
       <c r="EU29">
-        <v>5.920262151829601</v>
+        <v>5.920262151829602</v>
       </c>
       <c r="EV29">
         <v>1.500091024940834</v>
@@ -16953,13 +16953,13 @@
         <v>6.175131986164209</v>
       </c>
       <c r="FE29">
-        <v>4.61678499908975</v>
+        <v>4.616784999089751</v>
       </c>
       <c r="FF29">
         <v>28.45</v>
       </c>
       <c r="FG29">
-        <v>32.44</v>
+        <v>32.44000000000001</v>
       </c>
       <c r="FH29">
         <v>39.09</v>
@@ -17185,7 +17185,7 @@
         <v>4.472303206997085</v>
       </c>
       <c r="AV30">
-        <v>56.14681440443213</v>
+        <v>56.14681440443214</v>
       </c>
       <c r="AW30">
         <v>2.586846543001686</v>
@@ -17443,10 +17443,10 @@
         <v>54.15815341859448</v>
       </c>
       <c r="ED30">
-        <v>17.13440209979156</v>
+        <v>17.13440209979157</v>
       </c>
       <c r="EE30">
-        <v>28.95550809294665</v>
+        <v>28.95550809294666</v>
       </c>
       <c r="EF30">
         <v>29.87468155734541</v>
@@ -17530,7 +17530,7 @@
         <v>25.36000000000001</v>
       </c>
       <c r="FG30">
-        <v>39.19</v>
+        <v>39.19000000000001</v>
       </c>
       <c r="FH30">
         <v>35.45999999999999</v>
@@ -18198,7 +18198,7 @@
         <v>0.43</v>
       </c>
       <c r="F32">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="G32">
         <v>12.7</v>
@@ -18615,7 +18615,7 @@
         <v>0.3105621174325529</v>
       </c>
       <c r="EO32">
-        <v>7.160961340025445</v>
+        <v>7.160961340025446</v>
       </c>
       <c r="EP32">
         <v>7.699936885763231</v>
@@ -19147,7 +19147,7 @@
         <v>28.12005757645763</v>
       </c>
       <c r="EB33">
-        <v>62.25365628276437</v>
+        <v>62.25365628276438</v>
       </c>
       <c r="EC33">
         <v>47.85421072272671</v>
@@ -19775,7 +19775,7 @@
         <v>10.46173366756414</v>
       </c>
       <c r="EU34">
-        <v>9.621514560703122</v>
+        <v>9.621514560703123</v>
       </c>
       <c r="EV34">
         <v>0.5307461393247299</v>
@@ -19790,7 +19790,7 @@
         <v>11.13019527744252</v>
       </c>
       <c r="EZ34">
-        <v>0.6560826911769257</v>
+        <v>0.6560826911769258</v>
       </c>
       <c r="FA34">
         <v>0.3744622907189057</v>
@@ -19808,7 +19808,7 @@
         <v>7.048246835638906</v>
       </c>
       <c r="FF34">
-        <v>36.37</v>
+        <v>36.37000000000001</v>
       </c>
       <c r="FG34">
         <v>36.64000000000001</v>
@@ -20319,7 +20319,7 @@
         <v>5.094308967106332</v>
       </c>
       <c r="EL35">
-        <v>1.265084265099035</v>
+        <v>1.265084265099036</v>
       </c>
       <c r="EM35">
         <v>2.031667725211586</v>
@@ -20614,7 +20614,7 @@
         <v>2.124600638977636</v>
       </c>
       <c r="AX36">
-        <v>28.15823817292006</v>
+        <v>28.15823817292007</v>
       </c>
       <c r="AY36">
         <v>103.3592814371257</v>
@@ -20908,7 +20908,7 @@
         <v>2.413003787775567</v>
       </c>
       <c r="ER36">
-        <v>2.34624083712565</v>
+        <v>2.346240837125651</v>
       </c>
       <c r="ES36">
         <v>3.133771152955282</v>
@@ -20989,7 +20989,7 @@
         <v>2.94</v>
       </c>
       <c r="FS36">
-        <v>8.06</v>
+        <v>8.060000000000001</v>
       </c>
       <c r="FT36">
         <v>0</v>
@@ -21428,7 +21428,7 @@
         <v>10.25424075767294</v>
       </c>
       <c r="EA37">
-        <v>26.62226892476493</v>
+        <v>26.62226892476494</v>
       </c>
       <c r="EB37">
         <v>63.12349031756213</v>
@@ -22020,7 +22020,7 @@
         <v>4.88100793280448</v>
       </c>
       <c r="EI38">
-        <v>16.68561489840071</v>
+        <v>16.68561489840072</v>
       </c>
       <c r="EJ38">
         <v>0.4746956263521826</v>
@@ -22032,7 +22032,7 @@
         <v>1.989988546218131</v>
       </c>
       <c r="EM38">
-        <v>1.598863106095957</v>
+        <v>1.598863106095958</v>
       </c>
       <c r="EN38">
         <v>0.6498960675348916</v>
@@ -22128,7 +22128,7 @@
         <v>4.3</v>
       </c>
       <c r="FS38">
-        <v>7.56</v>
+        <v>7.560000000000001</v>
       </c>
       <c r="FT38">
         <v>0.83</v>
@@ -22609,7 +22609,7 @@
         <v>0.7980532337782077</v>
       </c>
       <c r="EO39">
-        <v>15.13429361708559</v>
+        <v>15.1342936170856</v>
       </c>
       <c r="EP39">
         <v>3.05315820498481</v>
@@ -22729,7 +22729,7 @@
         <v>23.07</v>
       </c>
       <c r="GC39">
-        <v>7.77</v>
+        <v>7.770000000000001</v>
       </c>
       <c r="GD39">
         <v>3.59</v>
@@ -23472,7 +23472,7 @@
         <v>21.32963549920761</v>
       </c>
       <c r="BA41">
-        <v>0.5813084112149532</v>
+        <v>0.5813084112149533</v>
       </c>
       <c r="BB41">
         <v>1.687979539641944</v>
@@ -24298,7 +24298,7 @@
         <v>46.55941821387251</v>
       </c>
       <c r="EH42">
-        <v>6.330229739408296</v>
+        <v>6.330229739408297</v>
       </c>
       <c r="EI42">
         <v>5.932639156703947</v>
@@ -24875,7 +24875,7 @@
         <v>5.92929044930027</v>
       </c>
       <c r="EJ43">
-        <v>0.3396349946804157</v>
+        <v>0.3396349946804158</v>
       </c>
       <c r="EK43">
         <v>0.3130370734102627</v>
@@ -24929,7 +24929,7 @@
         <v>0.7815696865537278</v>
       </c>
       <c r="FB43">
-        <v>1.231688354202471</v>
+        <v>1.231688354202472</v>
       </c>
       <c r="FC43">
         <v>2.94009329732384</v>
@@ -25437,7 +25437,7 @@
         <v>27.26964309947076</v>
       </c>
       <c r="EG44">
-        <v>45.54068200763817</v>
+        <v>45.54068200763818</v>
       </c>
       <c r="EH44">
         <v>4.856735746272997</v>
@@ -25765,7 +25765,7 @@
         <v>2.935374149659864</v>
       </c>
       <c r="BD45">
-        <v>1.081125827814569</v>
+        <v>1.08112582781457</v>
       </c>
       <c r="BE45">
         <v>65063380</v>
@@ -26002,7 +26002,7 @@
         <v>35.96528841245534</v>
       </c>
       <c r="EE45">
-        <v>25.47115875446656</v>
+        <v>25.47115875446657</v>
       </c>
       <c r="EF45">
         <v>21.55589586523737</v>
@@ -26035,7 +26035,7 @@
         <v>1.661051556916794</v>
       </c>
       <c r="EP45">
-        <v>4.325676365492598</v>
+        <v>4.325676365492599</v>
       </c>
       <c r="EQ45">
         <v>1.706993363961205</v>
@@ -26192,7 +26192,7 @@
         <v>19.6</v>
       </c>
       <c r="H46">
-        <v>79.46778</v>
+        <v>79.46778000000001</v>
       </c>
       <c r="I46">
         <v>78.60531</v>
@@ -26327,7 +26327,7 @@
         <v>70.52066115702479</v>
       </c>
       <c r="BA46">
-        <v>0.5155807365439093</v>
+        <v>0.5155807365439094</v>
       </c>
       <c r="BB46">
         <v>0.6905005107252298</v>
@@ -26582,7 +26582,7 @@
         <v>48.28361543376845</v>
       </c>
       <c r="EH46">
-        <v>0.569325601395208</v>
+        <v>0.5693256013952081</v>
       </c>
       <c r="EI46">
         <v>11.19673682743909</v>
@@ -26735,7 +26735,7 @@
         <v>16.11</v>
       </c>
       <c r="GG46">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="47">
@@ -26766,7 +26766,7 @@
         <v>77.75136000000002</v>
       </c>
       <c r="I47">
-        <v>66.02052</v>
+        <v>66.02052000000001</v>
       </c>
       <c r="J47">
         <v>9.11744</v>
@@ -27189,7 +27189,7 @@
         <v>2.658012218045113</v>
       </c>
       <c r="ET47">
-        <v>2.402490601503759</v>
+        <v>2.40249060150376</v>
       </c>
       <c r="EU47">
         <v>4.6062421679198</v>
@@ -27231,7 +27231,7 @@
         <v>39.88</v>
       </c>
       <c r="FH47">
-        <v>31.62</v>
+        <v>31.62000000000001</v>
       </c>
       <c r="FI47">
         <v>93.66999999999999</v>
@@ -27718,7 +27718,7 @@
         <v>36.6989649056494</v>
       </c>
       <c r="EF48">
-        <v>25.83592591515715</v>
+        <v>25.83592591515716</v>
       </c>
       <c r="EG48">
         <v>62.53489082080656</v>
@@ -27736,7 +27736,7 @@
         <v>0.3917948419736574</v>
       </c>
       <c r="EL48">
-        <v>1.320762945948303</v>
+        <v>1.320762945948304</v>
       </c>
       <c r="EM48">
         <v>0.8857180240165149</v>
@@ -27823,7 +27823,7 @@
         <v>2.04</v>
       </c>
       <c r="FO48">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="FP48">
         <v>0.09</v>
@@ -27908,7 +27908,7 @@
         <v>91.77210000000001</v>
       </c>
       <c r="I49">
-        <v>51.160205</v>
+        <v>51.16020500000001</v>
       </c>
       <c r="J49">
         <v>8.75342</v>
@@ -28325,7 +28325,7 @@
         <v>0.2788963100491083</v>
       </c>
       <c r="ER49">
-        <v>0.7804274266792049</v>
+        <v>0.780427426679205</v>
       </c>
       <c r="ES49">
         <v>2.399954990797225</v>
@@ -28842,7 +28842,7 @@
         <v>44225</v>
       </c>
       <c r="DZ50">
-        <v>12.78381795195954</v>
+        <v>12.78381795195955</v>
       </c>
       <c r="EA50">
         <v>36.91529709228824</v>
@@ -28965,7 +28965,7 @@
         <v>1.36</v>
       </c>
       <c r="FO50">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="FP50">
         <v>0.14</v>
@@ -29007,7 +29007,7 @@
         <v>24.62</v>
       </c>
       <c r="GC50">
-        <v>7.399999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="GD50">
         <v>4.46</v>
@@ -29458,7 +29458,7 @@
         <v>1.304802784718218</v>
       </c>
       <c r="EP51">
-        <v>0.7751937984496124</v>
+        <v>0.7751937984496125</v>
       </c>
       <c r="EQ51">
         <v>11.95464155295022</v>
@@ -29572,10 +29572,10 @@
         <v>24.88</v>
       </c>
       <c r="GC51">
-        <v>7.81</v>
+        <v>7.810000000000001</v>
       </c>
       <c r="GD51">
-        <v>4.27</v>
+        <v>4.270000000000001</v>
       </c>
       <c r="GE51">
         <v>0.11</v>
@@ -29729,7 +29729,7 @@
         <v>149.25</v>
       </c>
       <c r="AU52">
-        <v>2.183229813664596</v>
+        <v>2.183229813664597</v>
       </c>
       <c r="AV52">
         <v>32.71313672922252</v>
@@ -29984,7 +29984,7 @@
         <v>23.82002024836283</v>
       </c>
       <c r="EB52">
-        <v>57.86802680985762</v>
+        <v>57.86802680985763</v>
       </c>
       <c r="EC52">
         <v>33.22397508682446</v>
@@ -30050,7 +30050,7 @@
         <v>21.8220963463239</v>
       </c>
       <c r="EY52">
-        <v>8.855454883315605</v>
+        <v>8.855454883315606</v>
       </c>
       <c r="EZ52">
         <v>0.6061693429534416</v>
@@ -30543,7 +30543,7 @@
         <v>74524</v>
       </c>
       <c r="DZ53">
-        <v>10.0101498050169</v>
+        <v>10.01014980501691</v>
       </c>
       <c r="EA53">
         <v>26.19260208948618</v>
@@ -30594,7 +30594,7 @@
         <v>5.226768012088189</v>
       </c>
       <c r="EQ53">
-        <v>0.7745903828689606</v>
+        <v>0.7745903828689607</v>
       </c>
       <c r="ER53">
         <v>0.6051725848424491</v>
@@ -30606,7 +30606,7 @@
         <v>9.582026450544502</v>
       </c>
       <c r="EU53">
-        <v>2.249746254874577</v>
+        <v>2.249746254874578</v>
       </c>
       <c r="EV53">
         <v>1.144714851530484</v>
@@ -31138,7 +31138,7 @@
         <v>4.775355891040933</v>
       </c>
       <c r="EI54">
-        <v>7.574256999405772</v>
+        <v>7.574256999405773</v>
       </c>
       <c r="EJ54">
         <v>0.4951901960953176</v>
@@ -31150,13 +31150,13 @@
         <v>1.294384112576109</v>
       </c>
       <c r="EM54">
-        <v>0.3978745575583248</v>
+        <v>0.3978745575583249</v>
       </c>
       <c r="EN54">
         <v>0.4977737971184237</v>
       </c>
       <c r="EO54">
-        <v>10.95016233626428</v>
+        <v>10.95016233626429</v>
       </c>
       <c r="EP54">
         <v>5.585745411955183</v>

</xml_diff>